<commit_message>
Adding rudimentary implementation of chart commentaries.
</commit_message>
<xml_diff>
--- a/test/marine.xlsx
+++ b/test/marine.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="733" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="733" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary " sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Commentary" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>Water Quality</t>
   </si>
@@ -123,6 +124,30 @@
   </si>
   <si>
     <t>very poor</t>
+  </si>
+  <si>
+    <t>Commentary</t>
+  </si>
+  <si>
+    <t>This is a commentary about the Cape York region.</t>
+  </si>
+  <si>
+    <t>This is a commentary about the Wet Tropics region.</t>
+  </si>
+  <si>
+    <t>This is a commentary about the Burdekin region.</t>
+  </si>
+  <si>
+    <t>This is a commentary about the Mackay Whitsundays region.</t>
+  </si>
+  <si>
+    <t>This is a commentary about the Fitzroy region.</t>
+  </si>
+  <si>
+    <t>This is a commentary about the Burnett Mary region.</t>
+  </si>
+  <si>
+    <t>This is a commentary about the Great Barrier Reef region.</t>
   </si>
 </sst>
 </file>
@@ -314,7 +339,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -510,6 +535,18 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -520,83 +557,6 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -667,8 +627,8 @@
   </sheetPr>
   <dimension ref="A2:U26"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="H1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L14" activeCellId="0" pane="topLeft" sqref="L14"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1327,4 +1287,97 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3279352226721"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
+      <c r="A1" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="2">
+      <c r="A2" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="3">
+      <c r="A3" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="4">
+      <c r="A4" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="5">
+      <c r="A5" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="6">
+      <c r="A6" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="7">
+      <c r="A7" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="8">
+      <c r="A8" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing typo in example spreadsheet.
</commit_message>
<xml_diff>
--- a/test/marine.xlsx
+++ b/test/marine.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>Water Quality</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>This is a commentary about the Burdekin region.</t>
+  </si>
+  <si>
+    <t>Mackay Whitsunday</t>
   </si>
   <si>
     <t>This is a commentary about the Mackay Whitsundays region.</t>
@@ -1297,7 +1300,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1341,10 +1344,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="5">
       <c r="A5" s="50" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="6">
@@ -1352,7 +1355,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="7">
@@ -1360,7 +1363,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="8">
@@ -1368,7 +1371,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Markdown support for chart commentaries.
</commit_message>
<xml_diff>
--- a/test/marine.xlsx
+++ b/test/marine.xlsx
@@ -150,7 +150,10 @@
     <t>This is a commentary about the Burnett Mary region.</t>
   </si>
   <si>
-    <t>This is a commentary about the Great Barrier Reef region.</t>
+    <t>This is the *Great Barrier Reef* overview.
+ * Write in Markdown
+ * It's converted to HTML
+</t>
   </si>
 </sst>
 </file>
@@ -1300,13 +1303,13 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
+      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3279352226721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.1983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
@@ -1366,7 +1369,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.7" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="113.4" outlineLevel="0" r="8">
       <c r="A8" s="50" t="s">
         <v>23</v>
       </c>

</xml_diff>